<commit_message>
2 games max per week per team and no consecutive days
</commit_message>
<xml_diff>
--- a/volleyball_schedule.xlsx
+++ b/volleyball_schedule.xlsx
@@ -466,12 +466,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>動科 vs 工管</t>
+          <t>機械B vs 國企B</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>yoyo</t>
+          <t>恩臨</t>
         </is>
       </c>
     </row>
@@ -484,12 +484,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>機械B vs 國企B</t>
+          <t>機械A vs 人類哲學</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>恩臨</t>
+          <t>手槍</t>
         </is>
       </c>
     </row>
@@ -502,12 +502,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>農化生技 vs 生傳</t>
+          <t>國企A vs 生傳</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>大餅</t>
+          <t>yoyo</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>農藝 vs 化工A</t>
+          <t>物治職治 vs 會計</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -538,12 +538,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>土木B vs 森林</t>
+          <t>政治A vs 化工B</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>家葳</t>
+          <t>小馬</t>
         </is>
       </c>
     </row>
@@ -556,12 +556,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>護理 vs 機械A</t>
+          <t>經濟 vs 土木B</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>絲瓜</t>
+          <t>阿侑</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>阿侑</t>
+          <t>絲瓜</t>
         </is>
       </c>
     </row>
@@ -592,12 +592,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>土木A vs 會計</t>
+          <t>中文物理 vs 植微昆蟲</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>小馬</t>
+          <t>家葳</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>化學 vs 工管</t>
+          <t>法律 vs 森林</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -628,12 +628,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>材料資工 vs 政治A</t>
+          <t>生科 vs 物治職治</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>手槍</t>
+          <t>羿君</t>
         </is>
       </c>
     </row>
@@ -646,7 +646,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>社會社工 vs 人類哲學</t>
+          <t>外文 vs 日文戲劇</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -664,12 +664,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>法律 vs 土木B</t>
+          <t>農化生技 vs 國企A</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>羿君</t>
+          <t>手槍</t>
         </is>
       </c>
     </row>
@@ -682,12 +682,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>外文 vs 園藝</t>
+          <t>政治A vs 工海</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>家葳</t>
+          <t>阿宛</t>
         </is>
       </c>
     </row>
@@ -700,12 +700,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>農化生技 vs 藥學</t>
+          <t>材料資工 vs 化工B</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>阿宛</t>
+          <t>大餅</t>
         </is>
       </c>
     </row>
@@ -718,30 +718,30 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>材料資工 vs 化工B</t>
+          <t>化學 vs 工管</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>大餅</t>
+          <t>阿侑</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>土木A vs 生科</t>
+          <t>護理 vs 社會社工</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>yoyo</t>
+          <t>手槍</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -759,7 +759,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>阿宛</t>
+          <t>手槍</t>
         </is>
       </c>
     </row>
@@ -768,16 +768,16 @@
         <v>5</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>化工B vs 工海</t>
+          <t>法律 vs 經濟</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>大餅</t>
+          <t>yoyo</t>
         </is>
       </c>
     </row>
@@ -786,34 +786,34 @@
         <v>5</v>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>護理 vs 人類哲學</t>
+          <t>園藝 vs 地質地理</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>阿程</t>
+          <t>絲瓜</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>機械A vs 人類哲學</t>
+          <t>電機 vs 機械B</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>阿冠</t>
+          <t>阿程</t>
         </is>
       </c>
     </row>
@@ -822,16 +822,16 @@
         <v>6</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>國企A vs 藥學</t>
+          <t>社會社工 vs 人類哲學</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>茵茵</t>
+          <t>yoyo</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -849,7 +849,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>yoyo</t>
+          <t>阿冠</t>
         </is>
       </c>
     </row>
@@ -858,34 +858,34 @@
         <v>6</v>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>電機 vs 機械B</t>
+          <t>動科 vs 工管</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>恩臨</t>
+          <t>茵茵</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>外文 vs 日文戲劇</t>
+          <t>農化生技 vs 藥學</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>家葳</t>
+          <t>恩臨</t>
         </is>
       </c>
     </row>
@@ -894,16 +894,16 @@
         <v>7</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>化學 vs 政治B</t>
+          <t>土木A vs 物治職治</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>阿侑</t>
+          <t>家葳</t>
         </is>
       </c>
     </row>
@@ -912,16 +912,16 @@
         <v>7</v>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>財金 vs 化工A</t>
+          <t>化學 vs 政治B</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>小馬</t>
+          <t>阿侑</t>
         </is>
       </c>
     </row>
@@ -930,34 +930,34 @@
         <v>7</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>土木A vs 物治職治</t>
+          <t>土木B vs 森林</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>絲瓜</t>
+          <t>小馬</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>國企A vs 生傳</t>
+          <t>護理 vs 機械A</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>阿冠</t>
+          <t>絲瓜</t>
         </is>
       </c>
     </row>
@@ -966,11 +966,11 @@
         <v>8</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>政治A vs 工海</t>
+          <t>外文 vs 園藝</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -984,16 +984,16 @@
         <v>8</v>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>法律 vs 森林</t>
+          <t>農經生工 vs 機械B</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>羿君</t>
+          <t>阿冠</t>
         </is>
       </c>
     </row>
@@ -1002,34 +1002,34 @@
         <v>8</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>中文物理 vs 植微昆蟲</t>
+          <t>農藝 vs 財金</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>手槍</t>
+          <t>羿君</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>生科 vs 會計</t>
+          <t>材料資工 vs 工海</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>大餅</t>
+          <t>手槍</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>絲瓜</t>
+          <t>家葳</t>
         </is>
       </c>
     </row>
@@ -1056,11 +1056,11 @@
         <v>9</v>
       </c>
       <c r="B35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>護理 vs 社會社工</t>
+          <t>法律 vs 土木B</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1074,34 +1074,34 @@
         <v>9</v>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>經濟 vs 土木B</t>
+          <t>中文物理 vs 獸醫</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>芳芳</t>
+          <t>大餅</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>地質地理 vs 日文戲劇</t>
+          <t>生科 vs 會計</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>大餅</t>
+          <t>絲瓜</t>
         </is>
       </c>
     </row>
@@ -1110,11 +1110,11 @@
         <v>10</v>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>法律 vs 經濟</t>
+          <t>護理 vs 人類哲學</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1128,16 +1128,16 @@
         <v>10</v>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>農經生工 vs 機械B</t>
+          <t>園藝 vs 日文戲劇</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>小馬</t>
+          <t>阿宛</t>
         </is>
       </c>
     </row>
@@ -1146,34 +1146,34 @@
         <v>10</v>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>材料資工 vs 工海</t>
+          <t>化工B vs 工海</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>阿宛</t>
+          <t>大餅</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>電機 vs 國企B</t>
+          <t>外文 vs 地質地理</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>恩臨</t>
+          <t>小馬</t>
         </is>
       </c>
     </row>
@@ -1182,16 +1182,16 @@
         <v>11</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>物治職治 vs 會計</t>
+          <t>農藝 vs 化工A</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>小馬</t>
+          <t>恩臨</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
         <v>11</v>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>茵茵</t>
+          <t>阿侑</t>
         </is>
       </c>
     </row>
@@ -1218,34 +1218,34 @@
         <v>11</v>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>外文 vs 地質地理</t>
+          <t>生傳 vs 藥學</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>yoyo</t>
+          <t>茵茵</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>經濟 vs 森林</t>
+          <t>農經生工 vs 電機</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>阿侑</t>
+          <t>yoyo</t>
         </is>
       </c>
     </row>
@@ -1254,16 +1254,16 @@
         <v>12</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>政治A vs 化工B</t>
+          <t>經濟 vs 森林</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>小馬</t>
+          <t>阿侑</t>
         </is>
       </c>
     </row>
@@ -1272,16 +1272,16 @@
         <v>12</v>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>農化生技 vs 國企A</t>
+          <t>工管 vs 政治B</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>家葳</t>
+          <t>小馬</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>工管 vs 政治B</t>
+          <t>土木A vs 會計</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1312,12 +1312,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>生傳 vs 藥學</t>
+          <t>財金 vs 化工A</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>手槍</t>
+          <t>芳芳</t>
         </is>
       </c>
     </row>
@@ -1326,11 +1326,11 @@
         <v>13</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>農藝 vs 財金</t>
+          <t>地質地理 vs 日文戲劇</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1344,11 +1344,11 @@
         <v>13</v>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>生科 vs 物治職治</t>
+          <t>材料資工 vs 政治A</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1359,19 +1359,19 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>園藝 vs 日文戲劇</t>
+          <t>土木A vs 生科</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>芳芳</t>
+          <t>阿宛</t>
         </is>
       </c>
     </row>
@@ -1380,16 +1380,16 @@
         <v>14</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>園藝 vs 地質地理</t>
+          <t>國企A vs 藥學</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>家葳</t>
+          <t>芳芳</t>
         </is>
       </c>
     </row>
@@ -1398,16 +1398,16 @@
         <v>14</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>農經生工 vs 電機</t>
+          <t>農化生技 vs 生傳</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>阿侑</t>
+          <t>大餅</t>
         </is>
       </c>
     </row>
@@ -1416,16 +1416,16 @@
         <v>14</v>
       </c>
       <c r="B55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>中文物理 vs 獸醫</t>
+          <t>電機 vs 國企B</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>手槍</t>
+          <t>家葳</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -2153,7 +2153,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -2163,7 +2163,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -2183,7 +2183,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">

</xml_diff>